<commit_message>
Add some of ML stuff back
</commit_message>
<xml_diff>
--- a/ExcelFiles/Processed_With_Features_Uni.xlsx.xlsx
+++ b/ExcelFiles/Processed_With_Features_Uni.xlsx.xlsx
@@ -1029,10 +1029,10 @@
         <v>0.1569349788174618</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1335540567167593</v>
+        <v>1.267776705276705</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2250461479751917</v>
+        <v>0.1898159279031024</v>
       </c>
       <c r="R2" t="n">
         <v>-0.02768375777820477</v>
@@ -1384,7 +1384,7 @@
         <v>0.6288944756689877</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1903627335489217</v>
+        <v>3.0246900080915</v>
       </c>
       <c r="Q3" t="n">
         <v>1</v>
@@ -1739,10 +1739,10 @@
         <v>0.01660583941605839</v>
       </c>
       <c r="P4" t="n">
-        <v>0.3605634895913915</v>
+        <v>2.859020705128832</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.04748294500203489</v>
+        <v>0.04690211735636927</v>
       </c>
       <c r="R4" t="n">
         <v>-0.05432595573440644</v>
@@ -2094,10 +2094,10 @@
         <v>0.0164579236103923</v>
       </c>
       <c r="P5" t="n">
-        <v>0.3381986131868085</v>
+        <v>2.583451734794357</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.03904930062360247</v>
+        <v>0.03857029101609533</v>
       </c>
       <c r="R5" t="n">
         <v>-0.04903859349506717</v>
@@ -2449,10 +2449,10 @@
         <v>0.01731601731601732</v>
       </c>
       <c r="P6" t="n">
-        <v>0.3662317231882449</v>
+        <v>3.276398719245028</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.06660264219354284</v>
+        <v>0.06398425111214585</v>
       </c>
       <c r="R6" t="n">
         <v>-0.09020598329016745</v>
@@ -2804,7 +2804,7 @@
         <v>0.003632840881569387</v>
       </c>
       <c r="P7" t="n">
-        <v>0.4494502885528527</v>
+        <v>1.859342764515178</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -3159,10 +3159,10 @@
         <v>0.517987645852257</v>
       </c>
       <c r="P8" t="n">
-        <v>0.09478179707047819</v>
+        <v>1.819551714935018</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.7989886537371216</v>
+        <v>0.6590506613178531</v>
       </c>
       <c r="R8" t="n">
         <v>-0.0006780544480069564</v>
@@ -3514,10 +3514,10 @@
         <v>0.3543525644753157</v>
       </c>
       <c r="P9" t="n">
-        <v>0.02227538752941246</v>
+        <v>1.123605326361232</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.5451489628239728</v>
+        <v>0.4761398917672634</v>
       </c>
       <c r="R9" t="n">
         <v>0.01351539827729261</v>
@@ -3869,10 +3869,10 @@
         <v>0.4353963769620276</v>
       </c>
       <c r="P10" t="n">
-        <v>0.1764306612426229</v>
+        <v>2.280814031864804</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.6608170182349792</v>
+        <v>0.6478320852910183</v>
       </c>
       <c r="R10" t="n">
         <v>0.1051528589705226</v>
@@ -4224,10 +4224,10 @@
         <v>0.1873635461462124</v>
       </c>
       <c r="P11" t="n">
-        <v>0.2365029894275618</v>
+        <v>2.490448813454528</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.3604693735499511</v>
+        <v>0.3496859306819751</v>
       </c>
       <c r="R11" t="n">
         <v>-0.003793597732100862</v>
@@ -4579,10 +4579,10 @@
         <v>0.01988096745599595</v>
       </c>
       <c r="P12" t="n">
-        <v>0.3332184677833729</v>
+        <v>2.660344290594585</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.04613684712809839</v>
+        <v>0.04582657099298132</v>
       </c>
       <c r="R12" t="n">
         <v>-0.02921850291615701</v>
@@ -4934,10 +4934,10 @@
         <v>0.4719448997563656</v>
       </c>
       <c r="P13" t="n">
-        <v>0.1583968961071257</v>
+        <v>1.760032472358734</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.6613236281718285</v>
+        <v>0.6401687210225244</v>
       </c>
       <c r="R13" t="n">
         <v>0.008058718498168303</v>
@@ -5289,10 +5289,10 @@
         <v>0.1244363608806032</v>
       </c>
       <c r="P14" t="n">
-        <v>0.1058198851841163</v>
+        <v>1.331892594112016</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.1842941081490613</v>
+        <v>0.1753376953296858</v>
       </c>
       <c r="R14" t="n">
         <v>0.005115565698139674</v>
@@ -5644,10 +5644,10 @@
         <v>0.617167692864904</v>
       </c>
       <c r="P15" t="n">
-        <v>0.113451126876757</v>
+        <v>2.77461440380055</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.9504085996231691</v>
+        <v>0.8666025957380017</v>
       </c>
       <c r="R15" t="n">
         <v>0.04842918916299346</v>
@@ -5999,10 +5999,10 @@
         <v>0.5664138788140107</v>
       </c>
       <c r="P16" t="n">
-        <v>0.2339420610053731</v>
+        <v>1.212013047779471</v>
       </c>
       <c r="Q16" t="n">
-        <v>1</v>
+        <v>0.8923026910504533</v>
       </c>
       <c r="R16" t="n">
         <v>-0.01995005298608157</v>
@@ -6354,10 +6354,10 @@
         <v>0.4061757719714965</v>
       </c>
       <c r="P17" t="n">
-        <v>0.1363216715257531</v>
+        <v>2.081632653061224</v>
       </c>
       <c r="Q17" t="n">
-        <v>1</v>
+        <v>0.8596726074741664</v>
       </c>
       <c r="R17" t="n">
         <v>-0.00206904061853427</v>
@@ -6709,10 +6709,10 @@
         <v>0.4761508019162675</v>
       </c>
       <c r="P18" t="n">
-        <v>0.05962044798868996</v>
+        <v>1.031420765027322</v>
       </c>
       <c r="Q18" t="n">
-        <v>1</v>
+        <v>0.9814549083730499</v>
       </c>
       <c r="R18" t="n">
         <v>-0.0206563427473191</v>
@@ -7064,10 +7064,10 @@
         <v>0.3087757313109426</v>
       </c>
       <c r="P19" t="n">
-        <v>0.1660720104268491</v>
+        <v>1.678476996298255</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.7773579788060259</v>
+        <v>0.5773427603124879</v>
       </c>
       <c r="R19" t="n">
         <v>-0.03280970371843309</v>
@@ -7419,10 +7419,10 @@
         <v>0.3035204492042712</v>
       </c>
       <c r="P20" t="n">
-        <v>0.1655222936123148</v>
+        <v>1.379081350304372</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.4783638328035865</v>
+        <v>0.4384814313190686</v>
       </c>
       <c r="R20" t="n">
         <v>-0.004912515909392137</v>
@@ -7774,10 +7774,10 @@
         <v>0.03525523319867793</v>
       </c>
       <c r="P21" t="n">
-        <v>0.2421267014986938</v>
+        <v>9.197573070296954</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.1353165579695529</v>
+        <v>0.129449959608424</v>
       </c>
       <c r="R21" t="n">
         <v>0.0174618589543556</v>
@@ -8129,10 +8129,10 @@
         <v>0.5120611357976463</v>
       </c>
       <c r="P22" t="n">
-        <v>0.1109261882916064</v>
+        <v>1.792108384609682</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.8810691810146958</v>
+        <v>0.7732464799011314</v>
       </c>
       <c r="R22" t="n">
         <v>0.01914063480420137</v>
@@ -8484,10 +8484,10 @@
         <v>0.2877046165164613</v>
       </c>
       <c r="P23" t="n">
-        <v>0.07050244550507766</v>
+        <v>1.353399294670846</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.4605760756912376</v>
+        <v>0.4055382929463246</v>
       </c>
       <c r="R23" t="n">
         <v>-0.003843327008540067</v>
@@ -8839,10 +8839,10 @@
         <v>0.3297601265266673</v>
       </c>
       <c r="P24" t="n">
-        <v>0.1474228589413155</v>
+        <v>1.439061345158906</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.604456460126126</v>
+        <v>0.519847118453131</v>
       </c>
       <c r="R24" t="n">
         <v>-0.006192244273360301</v>
@@ -9194,10 +9194,10 @@
         <v>0.2606387109920022</v>
       </c>
       <c r="P25" t="n">
-        <v>0.04248550009095988</v>
+        <v>1.518065658733752</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.3748725936383752</v>
+        <v>0.3538648088358622</v>
       </c>
       <c r="R25" t="n">
         <v>0.002499374827629351</v>
@@ -9549,10 +9549,10 @@
         <v>0.2253112013012456</v>
       </c>
       <c r="P26" t="n">
-        <v>0.01588229576165942</v>
+        <v>1.380966311054348</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.3118354689768842</v>
+        <v>0.3018627052219365</v>
       </c>
       <c r="R26" t="n">
         <v>0.000821614119466078</v>
@@ -9904,10 +9904,10 @@
         <v>0.2645821668697685</v>
       </c>
       <c r="P27" t="n">
-        <v>0.234194348868247</v>
+        <v>3.131701744246485</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.3970575943521282</v>
+        <v>0.3928368265153722</v>
       </c>
       <c r="R27" t="n">
         <v>0.002994203672921123</v>
@@ -10259,10 +10259,10 @@
         <v>0.2223911602344453</v>
       </c>
       <c r="P28" t="n">
-        <v>0.02831206341687089</v>
+        <v>1.751920479207286</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.3090233317022339</v>
+        <v>0.3024426892435392</v>
       </c>
       <c r="R28" t="n">
         <v>0.001541028835222397</v>
@@ -10614,7 +10614,7 @@
         <v>0.3409090909090909</v>
       </c>
       <c r="P29" t="n">
-        <v>0.1719444444444444</v>
+        <v>1.042857142857143</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
@@ -10969,10 +10969,10 @@
         <v>0.4072398190045249</v>
       </c>
       <c r="P30" t="n">
-        <v>0.04727570738440304</v>
+        <v>1.254080854309688</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.856108092734684</v>
+        <v>0.662860537076067</v>
       </c>
       <c r="R30" t="n">
         <v>0.03234219538922969</v>
@@ -11324,10 +11324,10 @@
         <v>0.4072398190045249</v>
       </c>
       <c r="P31" t="n">
-        <v>0.04727570738440304</v>
+        <v>1.254080854309688</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.856108092734684</v>
+        <v>0.662860537076067</v>
       </c>
       <c r="R31" t="n">
         <v>0.03234219538922969</v>
@@ -11679,7 +11679,7 @@
         <v>0.002944062806673209</v>
       </c>
       <c r="P32" t="n">
-        <v>0.338784990027226</v>
+        <v>2.66304347826087</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -12034,10 +12034,10 @@
         <v>0.03538835935915636</v>
       </c>
       <c r="P33" t="n">
-        <v>0.2667735855550389</v>
+        <v>2.419900995904838</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.06583450304316622</v>
+        <v>0.06539438002334076</v>
       </c>
       <c r="R33" t="n">
         <v>-0.007937033739711842</v>
@@ -12389,10 +12389,10 @@
         <v>0.05177613941018767</v>
       </c>
       <c r="P34" t="n">
-        <v>0.3319753349988112</v>
+        <v>3.406183007532813</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.1711219580408752</v>
+        <v>0.1691913165499111</v>
       </c>
       <c r="R34" t="n">
         <v>-0.03415797574929064</v>
@@ -12744,10 +12744,10 @@
         <v>0.01114638384782216</v>
       </c>
       <c r="P35" t="n">
-        <v>0.3031059386942219</v>
+        <v>1.921213136929173</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.02126487703095944</v>
+        <v>0.02125223288369067</v>
       </c>
       <c r="R35" t="n">
         <v>-0.05172939191224014</v>
@@ -13099,10 +13099,10 @@
         <v>0.5202592721776538</v>
       </c>
       <c r="P36" t="n">
-        <v>0.04409140101016661</v>
+        <v>1.117520381479772</v>
       </c>
       <c r="Q36" t="n">
-        <v>1</v>
+        <v>0.81005129279212</v>
       </c>
       <c r="R36" t="n">
         <v>0.001355749924203857</v>
@@ -13454,10 +13454,10 @@
         <v>0.2583170254403131</v>
       </c>
       <c r="P37" t="n">
-        <v>0.1743055555555555</v>
+        <v>1.210338680926916</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.7805407399956806</v>
+        <v>0.5545895388809273</v>
       </c>
       <c r="R37" t="n">
         <v>-0.1013820431042814</v>
@@ -13809,10 +13809,10 @@
         <v>0.2556818181818182</v>
       </c>
       <c r="P38" t="n">
-        <v>0.1668985486351403</v>
+        <v>1.204099821746881</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.7566355676219659</v>
+        <v>0.5348344268794599</v>
       </c>
       <c r="R38" t="n">
         <v>-0.07774502579218864</v>
@@ -14164,7 +14164,7 @@
         <v>0.547243287558926</v>
       </c>
       <c r="P39" t="n">
-        <v>0.05079506987211983</v>
+        <v>0.9250693802035153</v>
       </c>
       <c r="Q39" t="n">
         <v>1</v>
@@ -14519,10 +14519,10 @@
         <v>0.5869961605170702</v>
       </c>
       <c r="P40" t="n">
-        <v>0.04498428592803382</v>
+        <v>1.75954312235209</v>
       </c>
       <c r="Q40" t="n">
-        <v>1</v>
+        <v>0.8416801054979732</v>
       </c>
       <c r="R40" t="n">
         <v>0.04930437724186707</v>
@@ -14874,7 +14874,7 @@
         <v>0.7395316909465335</v>
       </c>
       <c r="P41" t="n">
-        <v>0.0653575294243873</v>
+        <v>1.809684684684685</v>
       </c>
       <c r="Q41" t="n">
         <v>1</v>
@@ -15229,7 +15229,7 @@
         <v>0.7933130699088146</v>
       </c>
       <c r="P42" t="n">
-        <v>0.1007275132275132</v>
+        <v>1.049019607843137</v>
       </c>
       <c r="Q42" t="n">
         <v>0</v>
@@ -15584,7 +15584,7 @@
         <v>0.6632154394102543</v>
       </c>
       <c r="P43" t="n">
-        <v>0.08184893810557194</v>
+        <v>2.157569206749535</v>
       </c>
       <c r="Q43" t="n">
         <v>1</v>
@@ -15939,10 +15939,10 @@
         <v>0.3564206746669186</v>
       </c>
       <c r="P44" t="n">
-        <v>0.05373240477978396</v>
+        <v>1.459482972905792</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.5980292926959206</v>
+        <v>0.4957303650854569</v>
       </c>
       <c r="R44" t="n">
         <v>0.01829651407236406</v>
@@ -16294,10 +16294,10 @@
         <v>0.5426407133953399</v>
       </c>
       <c r="P45" t="n">
-        <v>0.05293367335817583</v>
+        <v>1.626436781609195</v>
       </c>
       <c r="Q45" t="n">
-        <v>1</v>
+        <v>0.7612297463794585</v>
       </c>
       <c r="R45" t="n">
         <v>0.03253346643236554</v>
@@ -16649,7 +16649,7 @@
         <v>0.6393258447643199</v>
       </c>
       <c r="P46" t="n">
-        <v>0.0118518679313113</v>
+        <v>0.9556841315761277</v>
       </c>
       <c r="Q46" t="n">
         <v>1</v>
@@ -17004,10 +17004,10 @@
         <v>0.6734384358806689</v>
       </c>
       <c r="P47" t="n">
-        <v>0.05710724856832101</v>
+        <v>1.520496660202543</v>
       </c>
       <c r="Q47" t="n">
-        <v>1</v>
+        <v>0.9642143711927134</v>
       </c>
       <c r="R47" t="n">
         <v>0.02419462968914022</v>
@@ -17359,10 +17359,10 @@
         <v>0.6057148742361477</v>
       </c>
       <c r="P48" t="n">
-        <v>0.01822745228770983</v>
+        <v>1.068830193830194</v>
       </c>
       <c r="Q48" t="n">
-        <v>1</v>
+        <v>0.9700791704754406</v>
       </c>
       <c r="R48" t="n">
         <v>0.006592017444729851</v>
@@ -17714,7 +17714,7 @@
         <v>0.6337080596512158</v>
       </c>
       <c r="P49" t="n">
-        <v>0.004277289089695161</v>
+        <v>0.7671435566626217</v>
       </c>
       <c r="Q49" t="n">
         <v>0</v>
@@ -18069,10 +18069,10 @@
         <v>0.2163009404388715</v>
       </c>
       <c r="P50" t="n">
-        <v>0.3008396913093046</v>
+        <v>3.960190300798036</v>
       </c>
       <c r="Q50" t="n">
-        <v>1</v>
+        <v>0.9403240161204618</v>
       </c>
       <c r="R50" t="n">
         <v>-0.01095560466285499</v>
@@ -18424,7 +18424,7 @@
         <v>0</v>
       </c>
       <c r="P51" t="n">
-        <v>0.1696135981404659</v>
+        <v>2.225040415438654</v>
       </c>
       <c r="Q51" t="n">
         <v>0</v>
@@ -18779,10 +18779,10 @@
         <v>0.3373083475298126</v>
       </c>
       <c r="P52" t="n">
-        <v>0.1945333880678708</v>
+        <v>1.076354679802956</v>
       </c>
       <c r="Q52" t="n">
-        <v>1</v>
+        <v>0.9286497374623692</v>
       </c>
       <c r="R52" t="n">
         <v>-0.09444044805261533</v>
@@ -19134,7 +19134,7 @@
         <v>0.5286624203821656</v>
       </c>
       <c r="P53" t="n">
-        <v>0.1596074380165289</v>
+        <v>0.9913419913419912</v>
       </c>
       <c r="Q53" t="n">
         <v>1</v>
@@ -19489,10 +19489,10 @@
         <v>0.3484031522189963</v>
       </c>
       <c r="P54" t="n">
-        <v>0.08144651581452823</v>
+        <v>1.53937728937729</v>
       </c>
       <c r="Q54" t="n">
-        <v>0.7165654850650076</v>
+        <v>0.5472060275151068</v>
       </c>
       <c r="R54" t="n">
         <v>-0.01984361310310165</v>
@@ -19844,10 +19844,10 @@
         <v>0.1031532245286009</v>
       </c>
       <c r="P55" t="n">
-        <v>0.2637411881771643</v>
+        <v>9.494592712222854</v>
       </c>
       <c r="Q55" t="n">
-        <v>0.3450450178910827</v>
+        <v>0.3416029413818354</v>
       </c>
       <c r="R55" t="n">
         <v>0.01128215174403742</v>
@@ -20199,10 +20199,10 @@
         <v>0.6055479270002044</v>
       </c>
       <c r="P56" t="n">
-        <v>0.0872067183078044</v>
+        <v>2.106837516984501</v>
       </c>
       <c r="Q56" t="n">
-        <v>0.8526654217342015</v>
+        <v>0.8244791884322085</v>
       </c>
       <c r="R56" t="n">
         <v>0.06818462167119203</v>
@@ -20554,7 +20554,7 @@
         <v>0.7253758328590083</v>
       </c>
       <c r="P57" t="n">
-        <v>0.01544242909970092</v>
+        <v>0.7223684210526317</v>
       </c>
       <c r="Q57" t="n">
         <v>0</v>
@@ -20909,10 +20909,10 @@
         <v>0.5216527100395694</v>
       </c>
       <c r="P58" t="n">
-        <v>0.0274925971199786</v>
+        <v>0.9740317460317459</v>
       </c>
       <c r="Q58" t="n">
-        <v>1</v>
+        <v>0.9524837190292864</v>
       </c>
       <c r="R58" t="n">
         <v>-0.0140787641351791</v>
@@ -21267,10 +21267,10 @@
         <v>0.4341438783077967</v>
       </c>
       <c r="P59" t="n">
-        <v>0.02892964495112788</v>
+        <v>1.073867163252638</v>
       </c>
       <c r="Q59" t="n">
-        <v>0.9120295118939183</v>
+        <v>0.6487455791348642</v>
       </c>
       <c r="R59" t="n">
         <v>-0.006544040617115356</v>
@@ -21625,7 +21625,7 @@
         <v>0.5880037219955623</v>
       </c>
       <c r="P60" t="n">
-        <v>0.02273020599011006</v>
+        <v>0.7989189189189189</v>
       </c>
       <c r="Q60" t="n">
         <v>0</v>
@@ -21982,7 +21982,7 @@
         <v>0.4952046348671977</v>
       </c>
       <c r="P61" t="n">
-        <v>0.02062220768918182</v>
+        <v>0.8281447534766118</v>
       </c>
       <c r="Q61" t="n">
         <v>1</v>
@@ -22341,7 +22341,7 @@
         <v>0.4952046348671977</v>
       </c>
       <c r="P62" t="n">
-        <v>0.02062220768918182</v>
+        <v>0.8281447534766119</v>
       </c>
       <c r="Q62" t="n">
         <v>1</v>
@@ -22700,10 +22700,10 @@
         <v>0.4356932876041156</v>
       </c>
       <c r="P63" t="n">
-        <v>0.06922247105754431</v>
+        <v>1.815427276522154</v>
       </c>
       <c r="Q63" t="n">
-        <v>0.7197514785206373</v>
+        <v>0.6366808221026278</v>
       </c>
       <c r="R63" t="n">
         <v>0.01212056729450505</v>
@@ -23055,7 +23055,7 @@
         <v>0.6684880047810126</v>
       </c>
       <c r="P64" t="n">
-        <v>0.02714048691369474</v>
+        <v>0.767345050878816</v>
       </c>
       <c r="Q64" t="n">
         <v>0</v>
@@ -23426,10 +23426,10 @@
         <v>0.3608815426997245</v>
       </c>
       <c r="P65" t="n">
-        <v>0.1862313537716764</v>
+        <v>1.47276573241671</v>
       </c>
       <c r="Q65" t="n">
-        <v>0.969181451053618</v>
+        <v>0.7659778325141647</v>
       </c>
       <c r="R65" t="n">
         <v>-0.05632903912067131</v>
@@ -23781,10 +23781,10 @@
         <v>0.05748865355521936</v>
       </c>
       <c r="P66" t="n">
-        <v>0.150787317035679</v>
+        <v>1.612186591793508</v>
       </c>
       <c r="Q66" t="n">
-        <v>0.06613520657002102</v>
+        <v>0.06091037900266594</v>
       </c>
       <c r="R66" t="n">
         <v>-0.01187752501484238</v>
@@ -24136,10 +24136,10 @@
         <v>0.108519003931848</v>
       </c>
       <c r="P67" t="n">
-        <v>0.1120971821086414</v>
+        <v>1.379251074278699</v>
       </c>
       <c r="Q67" t="n">
-        <v>0.1412655730337119</v>
+        <v>0.1260857798743614</v>
       </c>
       <c r="R67" t="n">
         <v>-0.004184175697147094</v>
@@ -24491,10 +24491,10 @@
         <v>0.1302352941176471</v>
       </c>
       <c r="P68" t="n">
-        <v>0.07490739755421601</v>
+        <v>1.222131326352531</v>
       </c>
       <c r="Q68" t="n">
-        <v>0.1559763208708439</v>
+        <v>0.1352162797270499</v>
       </c>
       <c r="R68" t="n">
         <v>-0.007746756092307463</v>
@@ -24846,10 +24846,10 @@
         <v>0.08906494147317635</v>
       </c>
       <c r="P69" t="n">
-        <v>0.05786986876343003</v>
+        <v>1.26642829153605</v>
       </c>
       <c r="Q69" t="n">
-        <v>0.09132556070321926</v>
+        <v>0.08233285725845652</v>
       </c>
       <c r="R69" t="n">
         <v>-0.005178154983436148</v>
@@ -25201,10 +25201,10 @@
         <v>0.1164132144729942</v>
       </c>
       <c r="P70" t="n">
-        <v>0.1067771876951616</v>
+        <v>1.401164172012355</v>
       </c>
       <c r="Q70" t="n">
-        <v>0.1561808398601473</v>
+        <v>0.1388263637141792</v>
       </c>
       <c r="R70" t="n">
         <v>0.005021575630382284</v>
@@ -25556,10 +25556,10 @@
         <v>0.1353062806926854</v>
       </c>
       <c r="P71" t="n">
-        <v>0.08555368457886878</v>
+        <v>1.244239391095819</v>
       </c>
       <c r="Q71" t="n">
-        <v>0.1650029888663652</v>
+        <v>0.1397045427471449</v>
       </c>
       <c r="R71" t="n">
         <v>-0.008825896390494369</v>
@@ -25911,10 +25911,10 @@
         <v>0.1707882534775889</v>
       </c>
       <c r="P72" t="n">
-        <v>0.05354419519097844</v>
+        <v>1.078856749311295</v>
       </c>
       <c r="Q72" t="n">
-        <v>0.18507261683236</v>
+        <v>0.1446989619491655</v>
       </c>
       <c r="R72" t="n">
         <v>-0.01088749470054045</v>
@@ -26266,10 +26266,10 @@
         <v>0.05572594928506631</v>
       </c>
       <c r="P73" t="n">
-        <v>0.07474184976159019</v>
+        <v>1.398521267821374</v>
       </c>
       <c r="Q73" t="n">
-        <v>0.05429005873490719</v>
+        <v>0.05057470682440842</v>
       </c>
       <c r="R73" t="n">
         <v>-0.004457973558076105</v>
@@ -26621,10 +26621,10 @@
         <v>0.1563786008230453</v>
       </c>
       <c r="P74" t="n">
-        <v>0.06491392972655673</v>
+        <v>1.164698787532534</v>
       </c>
       <c r="Q74" t="n">
-        <v>0.1994644979848535</v>
+        <v>0.1695692501307938</v>
       </c>
       <c r="R74" t="n">
         <v>-0.01905460461524048</v>
@@ -26976,10 +26976,10 @@
         <v>0.1021133715188623</v>
       </c>
       <c r="P75" t="n">
-        <v>0.06887907915825074</v>
+        <v>1.269757516063974</v>
       </c>
       <c r="Q75" t="n">
-        <v>0.1063903796338275</v>
+        <v>0.09327431662451528</v>
       </c>
       <c r="R75" t="n">
         <v>-0.001272320101468521</v>
@@ -27331,10 +27331,10 @@
         <v>0.09307760496413893</v>
       </c>
       <c r="P76" t="n">
-        <v>0.09362603307310151</v>
+        <v>1.39718875502008</v>
       </c>
       <c r="Q76" t="n">
-        <v>0.115538182082456</v>
+        <v>0.1052261129496151</v>
       </c>
       <c r="R76" t="n">
         <v>-0.008141776338248951</v>
@@ -27686,10 +27686,10 @@
         <v>0.083161059951137</v>
       </c>
       <c r="P77" t="n">
-        <v>0.1175840667382434</v>
+        <v>1.440664981230369</v>
       </c>
       <c r="Q77" t="n">
-        <v>0.0998341537045056</v>
+        <v>0.09097930875519861</v>
       </c>
       <c r="R77" t="n">
         <v>-0.01989725860302369</v>
@@ -28041,10 +28041,10 @@
         <v>0.09679427326486149</v>
       </c>
       <c r="P78" t="n">
-        <v>0.09410989449290386</v>
+        <v>1.310995015913049</v>
       </c>
       <c r="Q78" t="n">
-        <v>0.1030737376890146</v>
+        <v>0.0908424731566099</v>
       </c>
       <c r="R78" t="n">
         <v>-0.01230366555628395</v>
@@ -28396,10 +28396,10 @@
         <v>0.1478653245400902</v>
       </c>
       <c r="P79" t="n">
-        <v>0.08807077513836852</v>
+        <v>1.258064516129032</v>
       </c>
       <c r="Q79" t="n">
-        <v>0.1955011120575547</v>
+        <v>0.1638809397004752</v>
       </c>
       <c r="R79" t="n">
         <v>-0.01819319533296539</v>
@@ -28751,10 +28751,10 @@
         <v>0.07201516108654453</v>
       </c>
       <c r="P80" t="n">
-        <v>0.1832261447702624</v>
+        <v>1.636974789915966</v>
       </c>
       <c r="Q80" t="n">
-        <v>0.08781915724977277</v>
+        <v>0.07796485790404682</v>
       </c>
       <c r="R80" t="n">
         <v>-0.02210918205610233</v>
@@ -29106,10 +29106,10 @@
         <v>0.04992826398852224</v>
       </c>
       <c r="P81" t="n">
-        <v>0.1070074419054262</v>
+        <v>1.563624902182419</v>
       </c>
       <c r="Q81" t="n">
-        <v>0.05544195802065565</v>
+        <v>0.05222563824692394</v>
       </c>
       <c r="R81" t="n">
         <v>-0.01761298433306133</v>
@@ -29461,10 +29461,10 @@
         <v>0.2479338842975207</v>
       </c>
       <c r="P82" t="n">
-        <v>0.1036317951061189</v>
+        <v>1.112980769230769</v>
       </c>
       <c r="Q82" t="n">
-        <v>0.4654375794713052</v>
+        <v>0.3481747506837465</v>
       </c>
       <c r="R82" t="n">
         <v>-0.04260477445006546</v>
@@ -29816,10 +29816,10 @@
         <v>0.0548854041013269</v>
       </c>
       <c r="P83" t="n">
-        <v>0.2018326749911935</v>
+        <v>1.611264447127825</v>
       </c>
       <c r="Q83" t="n">
-        <v>0.06957808965418322</v>
+        <v>0.06469478630040321</v>
       </c>
       <c r="R83" t="n">
         <v>-0.02828600390779945</v>
@@ -30171,10 +30171,10 @@
         <v>0.0557361820715281</v>
       </c>
       <c r="P84" t="n">
-        <v>0.1954171472510573</v>
+        <v>1.419143752175426</v>
       </c>
       <c r="Q84" t="n">
-        <v>0.06672616380001893</v>
+        <v>0.06222534121177557</v>
       </c>
       <c r="R84" t="n">
         <v>-0.04550919503432575</v>
@@ -30526,10 +30526,10 @@
         <v>0.07761264449162539</v>
       </c>
       <c r="P85" t="n">
-        <v>0.127055093017374</v>
+        <v>1.276321974148061</v>
       </c>
       <c r="Q85" t="n">
-        <v>0.08544761605542618</v>
+        <v>0.07805510237765055</v>
       </c>
       <c r="R85" t="n">
         <v>-0.04574616567544494</v>
@@ -30881,10 +30881,10 @@
         <v>0.055003259452412</v>
       </c>
       <c r="P86" t="n">
-        <v>0.1284743852197261</v>
+        <v>1.553737191078963</v>
       </c>
       <c r="Q86" t="n">
-        <v>0.06523185802289287</v>
+        <v>0.0613189580632516</v>
       </c>
       <c r="R86" t="n">
         <v>-0.01534186414823019</v>
@@ -31236,10 +31236,10 @@
         <v>0.08760394507832141</v>
       </c>
       <c r="P87" t="n">
-        <v>0.2005143839348304</v>
+        <v>1.523037604965316</v>
       </c>
       <c r="Q87" t="n">
-        <v>0.1401901502913336</v>
+        <v>0.129683630497308</v>
       </c>
       <c r="R87" t="n">
         <v>-0.04150893321193847</v>
@@ -31591,10 +31591,10 @@
         <v>0.05801554310500633</v>
       </c>
       <c r="P88" t="n">
-        <v>0.2067861333648388</v>
+        <v>1.275161479741632</v>
       </c>
       <c r="Q88" t="n">
-        <v>0.06403079579582233</v>
+        <v>0.05943950903800611</v>
       </c>
       <c r="R88" t="n">
         <v>-0.04707827616534741</v>
@@ -31946,10 +31946,10 @@
         <v>0.1362907536076964</v>
       </c>
       <c r="P89" t="n">
-        <v>0.1006702676933556</v>
+        <v>1.254614325068871</v>
       </c>
       <c r="Q89" t="n">
-        <v>0.1759893400191765</v>
+        <v>0.149399947329996</v>
       </c>
       <c r="R89" t="n">
         <v>-0.01719945068568921</v>
@@ -32301,10 +32301,10 @@
         <v>0.04747180793015642</v>
       </c>
       <c r="P90" t="n">
-        <v>0.1133233085457777</v>
+        <v>1.51138811942136</v>
       </c>
       <c r="Q90" t="n">
-        <v>0.05323364962362059</v>
+        <v>0.05039572095042038</v>
       </c>
       <c r="R90" t="n">
         <v>-0.01063045840551168</v>
@@ -32656,10 +32656,10 @@
         <v>0.09506144215163459</v>
       </c>
       <c r="P91" t="n">
-        <v>0.1279203886238705</v>
+        <v>1.237733566339562</v>
       </c>
       <c r="Q91" t="n">
-        <v>0.1149690306788059</v>
+        <v>0.1042306915395538</v>
       </c>
       <c r="R91" t="n">
         <v>-0.03487661735937124</v>
@@ -33011,10 +33011,10 @@
         <v>0.1261089461901998</v>
       </c>
       <c r="P92" t="n">
-        <v>0.1142021970639511</v>
+        <v>1.391746353713899</v>
       </c>
       <c r="Q92" t="n">
-        <v>0.1780463769174904</v>
+        <v>0.1599559286812322</v>
       </c>
       <c r="R92" t="n">
         <v>-0.007142672270792536</v>
@@ -33366,10 +33366,10 @@
         <v>0.05261910405309315</v>
       </c>
       <c r="P93" t="n">
-        <v>0.1963507697862927</v>
+        <v>1.600821686658597</v>
       </c>
       <c r="Q93" t="n">
-        <v>0.07448570728902941</v>
+        <v>0.07042763344977761</v>
       </c>
       <c r="R93" t="n">
         <v>-0.03692831329363741</v>
@@ -33721,10 +33721,10 @@
         <v>0.04347155850161862</v>
       </c>
       <c r="P94" t="n">
-        <v>0.1543969619462869</v>
+        <v>1.533230457024479</v>
       </c>
       <c r="Q94" t="n">
-        <v>0.04596530731449294</v>
+        <v>0.04309680940171375</v>
       </c>
       <c r="R94" t="n">
         <v>-0.03840443720780393</v>
@@ -34076,10 +34076,10 @@
         <v>0.05562579013906448</v>
       </c>
       <c r="P95" t="n">
-        <v>0.2320651383502638</v>
+        <v>1.775314388371713</v>
       </c>
       <c r="Q95" t="n">
-        <v>0.08843674975920707</v>
+        <v>0.08203352838920465</v>
       </c>
       <c r="R95" t="n">
         <v>-0.03985567582570079</v>
@@ -34431,10 +34431,10 @@
         <v>0.1111539945966808</v>
       </c>
       <c r="P96" t="n">
-        <v>0.1485467290358595</v>
+        <v>1.464425770308123</v>
       </c>
       <c r="Q96" t="n">
-        <v>0.1631389042891919</v>
+        <v>0.143434184132826</v>
       </c>
       <c r="R96" t="n">
         <v>-0.03808325415371973</v>
@@ -34786,10 +34786,10 @@
         <v>0.05913978494623656</v>
       </c>
       <c r="P97" t="n">
-        <v>0.2681443375070826</v>
+        <v>1.701812555260831</v>
       </c>
       <c r="Q97" t="n">
-        <v>0.09641188427704066</v>
+        <v>0.08837209117538238</v>
       </c>
       <c r="R97" t="n">
         <v>-0.06367171629229787</v>
@@ -35141,10 +35141,10 @@
         <v>0.03883172917358115</v>
       </c>
       <c r="P98" t="n">
-        <v>0.1815431601053058</v>
+        <v>1.49207094160656</v>
       </c>
       <c r="Q98" t="n">
-        <v>0.05021821656606486</v>
+        <v>0.04834554504715814</v>
       </c>
       <c r="R98" t="n">
         <v>-0.04280644777249559</v>
@@ -35496,10 +35496,10 @@
         <v>0.1343283582089552</v>
       </c>
       <c r="P99" t="n">
-        <v>0.1758663734854211</v>
+        <v>1.313108038914491</v>
       </c>
       <c r="Q99" t="n">
-        <v>0.2089667857740292</v>
+        <v>0.1730706257416227</v>
       </c>
       <c r="R99" t="n">
         <v>-0.03992929187896433</v>
@@ -35851,10 +35851,10 @@
         <v>0.04327682426029272</v>
       </c>
       <c r="P100" t="n">
-        <v>0.1774941927990708</v>
+        <v>15.66337249196323</v>
       </c>
       <c r="Q100" t="n">
-        <v>0.1119159391271508</v>
+        <v>0.1082323952742092</v>
       </c>
       <c r="R100" t="n">
         <v>0.01962341410731602</v>
@@ -36202,10 +36202,10 @@
         <v>0.02905569007263923</v>
       </c>
       <c r="P101" t="n">
-        <v>0.2201984126984127</v>
+        <v>4.50248348143085</v>
       </c>
       <c r="Q101" t="n">
-        <v>0.04445994857992465</v>
+        <v>0.03884586031752917</v>
       </c>
       <c r="R101" t="n">
         <v>0.1155415099824639</v>
@@ -36553,10 +36553,10 @@
         <v>0.02870813397129187</v>
       </c>
       <c r="P102" t="n">
-        <v>0.2170209488601355</v>
+        <v>7.042363250496338</v>
       </c>
       <c r="Q102" t="n">
-        <v>0.0735641257509724</v>
+        <v>0.06826133340596426</v>
       </c>
       <c r="R102" t="n">
         <v>0.06334077395650207</v>
@@ -36904,10 +36904,10 @@
         <v>0.06507592190889371</v>
       </c>
       <c r="P103" t="n">
-        <v>0.2554469273743016</v>
+        <v>4.734699642207017</v>
       </c>
       <c r="Q103" t="n">
-        <v>0.2318135795171408</v>
+        <v>0.2017788749790174</v>
       </c>
       <c r="R103" t="n">
         <v>0.03684049024385849</v>
@@ -37255,10 +37255,10 @@
         <v>0.03773974015260879</v>
       </c>
       <c r="P104" t="n">
-        <v>0.182525623885918</v>
+        <v>10.98275803480407</v>
       </c>
       <c r="Q104" t="n">
-        <v>0.097818666596466</v>
+        <v>0.09356327816958909</v>
       </c>
       <c r="R104" t="n">
         <v>0.02555200180889534</v>
@@ -37606,10 +37606,10 @@
         <v>0.0821917808219178</v>
       </c>
       <c r="P105" t="n">
-        <v>0.32421875</v>
+        <v>1.985887096774194</v>
       </c>
       <c r="Q105" t="n">
-        <v>0.356582985712889</v>
+        <v>0.2692790137576984</v>
       </c>
       <c r="R105" t="n">
         <v>-0.2203389830508475</v>
@@ -37957,10 +37957,10 @@
         <v>0.02866242038216561</v>
       </c>
       <c r="P106" t="n">
-        <v>0.3167134831460674</v>
+        <v>5.09833047673459</v>
       </c>
       <c r="Q106" t="n">
-        <v>0.2815281105923315</v>
+        <v>0.2491633229525508</v>
       </c>
       <c r="R106" t="n">
         <v>-0.04961970300615726</v>
@@ -38308,10 +38308,10 @@
         <v>0.01989150090415913</v>
       </c>
       <c r="P107" t="n">
-        <v>0.2023736338797814</v>
+        <v>6.921950213754334</v>
       </c>
       <c r="Q107" t="n">
-        <v>0.04025831955191196</v>
+        <v>0.03693767076136182</v>
       </c>
       <c r="R107" t="n">
         <v>0.1028425317705463</v>
@@ -38659,7 +38659,7 @@
         <v>0.003690036900369004</v>
       </c>
       <c r="P108" t="n">
-        <v>0.2476041666666667</v>
+        <v>4.754218967921897</v>
       </c>
       <c r="Q108" t="n">
         <v>0</v>
@@ -39010,10 +39010,10 @@
         <v>0.02748091603053435</v>
       </c>
       <c r="P109" t="n">
-        <v>0.2467592592592593</v>
+        <v>5.375339910200468</v>
       </c>
       <c r="Q109" t="n">
-        <v>0.07127932225515933</v>
+        <v>0.06368807331603185</v>
       </c>
       <c r="R109" t="n">
         <v>0.01315400664416126</v>
@@ -39361,10 +39361,10 @@
         <v>0.03348837209302326</v>
       </c>
       <c r="P110" t="n">
-        <v>0.168010752688172</v>
+        <v>4.665436855165209</v>
       </c>
       <c r="Q110" t="n">
-        <v>0.05377850632984012</v>
+        <v>0.04717318684897186</v>
       </c>
       <c r="R110" t="n">
         <v>0.1768456572301436</v>
@@ -39712,10 +39712,10 @@
         <v>0.04943625325238508</v>
       </c>
       <c r="P111" t="n">
-        <v>0.2143034825870646</v>
+        <v>5.661381714183572</v>
       </c>
       <c r="Q111" t="n">
-        <v>0.1254405963680818</v>
+        <v>0.1133641017658893</v>
       </c>
       <c r="R111" t="n">
         <v>0.006810329743471909</v>
@@ -40063,10 +40063,10 @@
         <v>0.05587892898719441</v>
       </c>
       <c r="P112" t="n">
-        <v>0.1914036346245815</v>
+        <v>7.685839558699847</v>
       </c>
       <c r="Q112" t="n">
-        <v>0.1386969068952801</v>
+        <v>0.1294035631678835</v>
       </c>
       <c r="R112" t="n">
         <v>0.1328781913307239</v>
@@ -40414,7 +40414,7 @@
         <v>0.004195804195804196</v>
       </c>
       <c r="P113" t="n">
-        <v>0.2084319526627219</v>
+        <v>4.332769794308255</v>
       </c>
       <c r="Q113" t="n">
         <v>0</v>
@@ -40765,7 +40765,7 @@
         <v>0.002540220152413209</v>
       </c>
       <c r="P114" t="n">
-        <v>0.1714754566210046</v>
+        <v>7.489834700063441</v>
       </c>
       <c r="Q114" t="n">
         <v>0</v>
@@ -41116,10 +41116,10 @@
         <v>0.03894772804919713</v>
       </c>
       <c r="P115" t="n">
-        <v>0.1942462600690449</v>
+        <v>9.034133995853065</v>
       </c>
       <c r="Q115" t="n">
-        <v>0.09921939452441096</v>
+        <v>0.09313911187776423</v>
       </c>
       <c r="R115" t="n">
         <v>0.03327459983232932</v>
@@ -41467,10 +41467,10 @@
         <v>0.03804573804573805</v>
       </c>
       <c r="P116" t="n">
-        <v>0.2486458333333333</v>
+        <v>17.13404260349434</v>
       </c>
       <c r="Q116" t="n">
-        <v>0.133025825271664</v>
+        <v>0.1266601345663992</v>
       </c>
       <c r="R116" t="n">
         <v>-9.592054633838462e-05</v>
@@ -41818,10 +41818,10 @@
         <v>0.01336728198599618</v>
       </c>
       <c r="P117" t="n">
-        <v>0.2074054246966453</v>
+        <v>6.58480300704892</v>
       </c>
       <c r="Q117" t="n">
-        <v>0.02093326422366519</v>
+        <v>0.01923686597750026</v>
       </c>
       <c r="R117" t="n">
         <v>0.1079175797108836</v>
@@ -42169,7 +42169,7 @@
         <v>0</v>
       </c>
       <c r="P118" t="n">
-        <v>0.2921597633136095</v>
+        <v>4.724394195548042</v>
       </c>
       <c r="Q118" t="n">
         <v>0</v>
@@ -42520,10 +42520,10 @@
         <v>0.03703703703703703</v>
       </c>
       <c r="P119" t="n">
-        <v>0.2196862599206349</v>
+        <v>4.277514179755673</v>
       </c>
       <c r="Q119" t="n">
-        <v>0.06282551611885671</v>
+        <v>0.05441094612795219</v>
       </c>
       <c r="R119" t="n">
         <v>0.1057749835217766</v>
@@ -42871,10 +42871,10 @@
         <v>0.0469361147327249</v>
       </c>
       <c r="P120" t="n">
-        <v>0.1868628789469999</v>
+        <v>28.51650910143887</v>
       </c>
       <c r="Q120" t="n">
-        <v>0.1188405546268365</v>
+        <v>0.1166410263465589</v>
       </c>
       <c r="R120" t="n">
         <v>0.1689545046479095</v>
@@ -43226,10 +43226,10 @@
         <v>0.03341930831738636</v>
       </c>
       <c r="P121" t="n">
-        <v>0.2553289491655057</v>
+        <v>100.9440372241193</v>
       </c>
       <c r="Q121" t="n">
-        <v>0.1462770851364744</v>
+        <v>0.1448057673204027</v>
       </c>
       <c r="R121" t="n">
         <v>0.1016586182564275</v>
@@ -43581,10 +43581,10 @@
         <v>0.4692859957098455</v>
       </c>
       <c r="P122" t="n">
-        <v>0.08381101085779182</v>
+        <v>1.716668997404141</v>
       </c>
       <c r="Q122" t="n">
-        <v>0.7371609766763523</v>
+        <v>0.6683724048296448</v>
       </c>
       <c r="R122" t="n">
         <v>0.0110817360464814</v>
@@ -43936,7 +43936,7 @@
         <v>0.843065693430657</v>
       </c>
       <c r="P123" t="n">
-        <v>0.08581527168483692</v>
+        <v>0.9308300395256918</v>
       </c>
       <c r="Q123" t="n">
         <v>0</v>

</xml_diff>